<commit_message>
Add empty uploads folder
</commit_message>
<xml_diff>
--- a/uploads/exdata.xlsx
+++ b/uploads/exdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rizaf\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project1\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5044D8F-12B7-4626-9F68-2ACD4628C637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C534B45C-D627-463E-916E-FBC9CD7FA039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4356" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,29 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Widget A</t>
-  </si>
-  <si>
-    <t>Widget B</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Widget C</t>
-  </si>
-  <si>
-    <t>Widget D</t>
-  </si>
-  <si>
-    <t>Widget E</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,7 +377,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,72 +389,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>50</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>30</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>20</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>40</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>60</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>

</xml_diff>